<commit_message>
ID:OMS-SIQ-02-->Update SIQ after finish SRS
</commit_message>
<xml_diff>
--- a/Requirement/OnlineMobileStore_SIQ.xlsx
+++ b/Requirement/OnlineMobileStore_SIQ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E130DBE-0858-4EAF-94DE-F93774CCE75D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6AA0C1-227D-4844-8A48-1395F205127B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AB0B20E0-7525-4110-ADC5-AB52DD2125F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,18 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
   <si>
     <t>Question ID</t>
   </si>
@@ -103,52 +97,52 @@
     <t>The Supplier will register using full name, email, gender, and birthday. Yes or no?</t>
   </si>
   <si>
-    <t>Admin-P_01</t>
-  </si>
-  <si>
-    <t>Admin-P_02</t>
-  </si>
-  <si>
-    <t>Core-B_01</t>
-  </si>
-  <si>
-    <t>Core-B_02</t>
-  </si>
-  <si>
-    <t>Core-B_03</t>
-  </si>
-  <si>
-    <t>Core-B_04</t>
-  </si>
-  <si>
-    <t>Core-B_05</t>
-  </si>
-  <si>
-    <t>Core-B_06</t>
-  </si>
-  <si>
-    <t>Hist_01</t>
-  </si>
-  <si>
-    <t>Hist_02</t>
-  </si>
-  <si>
-    <t>Log_01</t>
-  </si>
-  <si>
-    <t>Log_02</t>
-  </si>
-  <si>
-    <t>Log_03</t>
-  </si>
-  <si>
-    <t>Log_04</t>
-  </si>
-  <si>
-    <t>Reg_01</t>
-  </si>
-  <si>
-    <t>Reg_02</t>
+    <t>OMS_SIQ_admin_01</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_admin_02</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_client_03</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_client_04</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_client_05</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_client_06</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_client_07</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_client_08</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_hist_10</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_hist_11</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_hist_12</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_Log_13</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_Log_14</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_Log_15</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_Reg_18</t>
+  </si>
+  <si>
+    <t>OMS_SIQ_Reg_19</t>
   </si>
   <si>
     <t>Delete user &amp; items only</t>
@@ -157,7 +151,7 @@
     <t>Can Client buy products on cash or by visa as the 2 only available payment method?</t>
   </si>
   <si>
-    <t>Core-B_07</t>
+    <t>OMS_SIQ_client_09</t>
   </si>
   <si>
     <t>the client will see the total cost of the cart and able to edit (edit quantity or remove items) the cart before submission?</t>
@@ -175,13 +169,13 @@
     <t>when user login using wrong password the website will display generic error msg that state "password or username is wrong"?</t>
   </si>
   <si>
-    <t>Log_05</t>
+    <t>OMS_SIQ_Log_16</t>
   </si>
   <si>
     <t>The constrains of the Strong password will be 8 characters (including at least 1 special characters, and at least 1 number)</t>
   </si>
   <si>
-    <t>Log_06</t>
+    <t>OMS_SIQ_Log_17</t>
   </si>
   <si>
     <t>Will the user have "forget password option" which help him regain access to his/her account again?</t>
@@ -200,21 +194,19 @@
   </si>
   <si>
     <t>Feature Category</t>
+  </si>
+  <si>
+    <t>Incorrect username or password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -263,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -272,10 +264,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -284,43 +276,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -335,9 +298,36 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{3ADA4072-798F-4876-AB09-88D256FF830C}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -351,8 +341,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1BD281A6-575E-48B7-AE98-1497DC4E72A4}" name="Table1" displayName="Table1" ref="A1:E20" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:E20" xr:uid="{1BD281A6-575E-48B7-AE98-1497DC4E72A4}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E20" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:E20" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="3">
       <filters>
         <filter val="Registration"/>
@@ -360,14 +350,14 @@
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E19">
-    <sortCondition ref="D1:D19"/>
+    <sortCondition ref="D2:D19"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{EFE33F09-CD36-4753-854C-EE3045504C97}" name="Question ID" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{13F49A65-B951-42B7-B093-B09927ABB880}" name="Question" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{39C08CE0-F1C4-4182-A47D-98B457B915FB}" name="Response" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{2309FEC9-3A41-4931-8495-D031904F1EC0}" name="Feature Category"/>
-    <tableColumn id="5" xr3:uid="{8A62B91B-7603-47BB-B7CF-A3C06CDDE756}" name="Additional info" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Question ID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Question" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Response" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Feature Category"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Additional info" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -672,20 +662,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A0F32C-55F4-4028-8167-824D8CFEA78E}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="66.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="66.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -702,7 +692,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
@@ -719,7 +709,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
@@ -734,7 +724,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
@@ -749,7 +739,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>26</v>
       </c>
@@ -764,7 +754,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -779,7 +769,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
@@ -796,7 +786,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
@@ -811,7 +801,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
@@ -826,7 +816,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>41</v>
       </c>
@@ -838,7 +828,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
@@ -853,7 +843,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -870,7 +860,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
@@ -885,22 +875,24 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>35</v>
       </c>
@@ -915,19 +907,22 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="C16" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="D16" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
@@ -944,7 +939,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>49</v>
       </c>
@@ -959,7 +954,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
@@ -976,7 +971,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>38</v>
       </c>
@@ -994,12 +989,11 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1011,7 +1005,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AD094658-2B17-4B08-B91C-85D984E4074F}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$2</xm:f>
           </x14:formula1>
@@ -1031,14 +1025,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
ID:OMS-SIQ-02-->Update SIQ and approved
</commit_message>
<xml_diff>
--- a/Requirement/OnlineMobileStore_SIQ.xlsx
+++ b/Requirement/OnlineMobileStore_SIQ.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\My Lab\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6AA0C1-227D-4844-8A48-1395F205127B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C414CD2F-6775-44B8-A64C-939BCFEB6C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
   <si>
     <t>Question ID</t>
   </si>
@@ -196,14 +196,23 @@
     <t>Feature Category</t>
   </si>
   <si>
-    <t>Incorrect username or password</t>
+    <t>OMS_SIQ_QUES_20</t>
+  </si>
+  <si>
+    <t>there is a conflict between OMS_SIQ_client_06 and OMS_SIQ_Reg_19, the corporate does not have a gender, I suggest using only supplier "person" instead of corporate </t>
+  </si>
+  <si>
+    <t>OMS_SIQ_QUES_21</t>
+  </si>
+  <si>
+    <t>there is an ambiguity in OMS_SIQ_admin_01, shall we use the item id to delete it?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -222,8 +231,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,8 +269,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -251,11 +296,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -276,8 +339,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -308,7 +395,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -406,7 +492,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -458,7 +544,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -659,23 +745,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A0F32C-55F4-4028-8167-824D8CFEA78E}">
-  <dimension ref="A1:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="109" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="2" max="2" width="66.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="26.27734375" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="25.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -692,7 +778,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
@@ -709,7 +795,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
@@ -724,7 +810,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
@@ -739,7 +825,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>26</v>
       </c>
@@ -754,7 +840,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
@@ -769,7 +855,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
@@ -786,7 +872,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
@@ -801,7 +887,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
@@ -816,7 +902,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A10" s="7" t="s">
         <v>41</v>
       </c>
@@ -828,7 +914,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
@@ -843,7 +929,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="36.9" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -860,7 +946,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
@@ -875,24 +961,22 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
         <v>35</v>
       </c>
@@ -907,7 +991,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
@@ -922,7 +1006,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="86.1" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
@@ -939,7 +1023,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
         <v>49</v>
       </c>
@@ -954,7 +1038,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
@@ -971,14 +1055,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D20" t="s">
@@ -988,8 +1072,38 @@
         <v>52</v>
       </c>
     </row>
+    <row r="21" spans="1:5" ht="36.9" x14ac:dyDescent="0.4">
+      <c r="A21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" ht="24.9" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="13"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C1:C20 C22:C1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
@@ -1009,7 +1123,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C20</xm:sqref>
+          <xm:sqref>C2:C22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1018,21 +1132,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D52817-3EC2-428C-AA53-A91F7D90B002}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>21</v>
       </c>

</xml_diff>